<commit_message>
Working on presentation materials.
</commit_message>
<xml_diff>
--- a/Presentation Materials/Data_Vis.xlsx
+++ b/Presentation Materials/Data_Vis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Learning\AMMRP\AMMRP-Course-Project\Presentation Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CFF0B0B-96AC-48AA-A58C-6193D386BD24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6244EF5-972B-41AE-AFF1-7FD0EB8E184F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{07B9CE15-5DA7-4058-82CC-C08E39CE511A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Uncalibrated</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Z</t>
   </si>
   <si>
-    <t>Calibrated</t>
-  </si>
-  <si>
     <t>&gt;</t>
   </si>
   <si>
@@ -58,12 +55,36 @@
   <si>
     <t>Norms After Calibration</t>
   </si>
+  <si>
+    <t>Norms After Calibration (LSM)</t>
+  </si>
+  <si>
+    <t>Norms After Calibration (NM)</t>
+  </si>
+  <si>
+    <t>M Matrix Values (LSM)</t>
+  </si>
+  <si>
+    <t>M Matrix Values (NM)</t>
+  </si>
+  <si>
+    <t>B Matrix Values (LSM)</t>
+  </si>
+  <si>
+    <t>B Matrix Values (NM)</t>
+  </si>
+  <si>
+    <t>Calibrated (LSM)</t>
+  </si>
+  <si>
+    <t>Calibrated (NM)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,8 +123,29 @@
       <color theme="1"/>
       <name val="Montserrat"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Montserrat Black"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Montserrat ExtraBold"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,8 +164,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -157,45 +211,127 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="40% - Accent2" xfId="1" builtinId="35"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF5AC72"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -504,226 +640,845 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A01563-FFE2-409C-9FDC-6DA6778B0B8D}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:S61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="18.42578125" customWidth="1"/>
+    <col min="1" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="7" width="20" customWidth="1"/>
     <col min="9" max="11" width="14.42578125" customWidth="1"/>
     <col min="12" max="12" width="18.140625" customWidth="1"/>
     <col min="13" max="15" width="14.42578125" customWidth="1"/>
+    <col min="17" max="17" width="39.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21.75" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:19" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="8" t="s">
+      <c r="M1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-    </row>
-    <row r="2" spans="1:15" ht="21.75" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="Q1" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+    </row>
+    <row r="2" spans="1:19" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="25" t="s">
         <v>3</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="9">
+      <c r="I2" s="4">
         <v>9.7183700000000002</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="9">
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="4">
         <v>9.7978900000000007</v>
       </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-    </row>
-    <row r="3" spans="1:15" ht="21.75" x14ac:dyDescent="0.4">
-      <c r="A3" s="6">
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="Q2" s="13">
+        <v>-5.5873600000000002E-2</v>
+      </c>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+    </row>
+    <row r="3" spans="1:19" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="A3" s="3">
         <v>0.68614398499999996</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="3">
         <v>9.6930132409999992</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="3">
         <v>0.14623097299999999</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="6">
+      <c r="D3" s="9"/>
+      <c r="E3" s="22">
         <v>-0.21872</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="22">
         <v>9.7875599999999991</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="22">
         <v>0.39309699999999997</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="9">
+      <c r="I3" s="4">
         <v>9.5608500000000003</v>
       </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="9">
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="4">
         <v>9.7950400000000002</v>
       </c>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-    </row>
-    <row r="4" spans="1:15" ht="21.75" x14ac:dyDescent="0.4">
-      <c r="A4" s="6">
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+    </row>
+    <row r="4" spans="1:19" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="A4" s="3">
         <v>0.30731318400000002</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="3">
         <v>-9.5551318219999999</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>0.12170737099999999</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="6">
+      <c r="D4" s="9"/>
+      <c r="E4" s="22">
         <v>0.23227</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="22">
         <v>-9.7922799999999999</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="22">
         <v>-4.1399599999999998E-3</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="9">
+      <c r="I4" s="4">
         <v>10.2112</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="9">
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="4">
         <v>9.7962100000000003</v>
       </c>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-    </row>
-    <row r="5" spans="1:15" ht="21.75" x14ac:dyDescent="0.4">
-      <c r="A5" s="6">
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="Q4" s="13">
+        <v>-0.35741000000000001</v>
+      </c>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+    </row>
+    <row r="5" spans="1:19" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="A5" s="3">
         <v>10.205881659999999</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="3">
         <v>0.14662737200000001</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="3">
         <v>0.29391314200000002</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="6">
+      <c r="D5" s="9"/>
+      <c r="E5" s="22">
         <v>9.7751999999999999</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="22">
         <v>0.45821600000000001</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="22">
         <v>0.44861400000000001</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="9">
+      <c r="I5" s="4">
         <v>9.2382200000000001</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="9">
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="4">
         <v>9.7976500000000009</v>
       </c>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-    </row>
-    <row r="6" spans="1:15" ht="21.75" x14ac:dyDescent="0.4">
-      <c r="A6" s="6">
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+    </row>
+    <row r="6" spans="1:19" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="A6" s="3">
         <v>-9.2357303369999997</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="3">
         <v>0.14983565600000001</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>-0.153514714</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="6">
+      <c r="D6" s="9"/>
+      <c r="E6" s="22">
         <v>-9.7913300000000003</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="22">
         <v>-0.29977199999999998</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="22">
         <v>-0.18428</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="9">
+      <c r="I6" s="4">
         <v>9.72837</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="9">
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="4">
         <v>9.7833600000000001</v>
       </c>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-    </row>
-    <row r="7" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="Q6" s="13">
+        <v>0.33792899999999998</v>
+      </c>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+    </row>
+    <row r="7" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
       <c r="H7" s="1"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+    </row>
+    <row r="8" spans="1:19" ht="21.75" x14ac:dyDescent="0.25">
+      <c r="E8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:19" ht="21.75" x14ac:dyDescent="0.25">
+      <c r="E9" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="E10" s="22">
+        <v>-0.21872</v>
+      </c>
+      <c r="F10" s="22">
+        <v>9.7875599999999991</v>
+      </c>
+      <c r="G10" s="22">
+        <v>0.39309699999999997</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="O10" s="13">
+        <v>-0.488037</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="E11" s="22">
+        <v>0.23227</v>
+      </c>
+      <c r="F11" s="22">
+        <v>-9.7922799999999999</v>
+      </c>
+      <c r="G11" s="22">
+        <v>-4.1399599999999998E-3</v>
+      </c>
+      <c r="I11" s="4">
+        <v>9.7957699999999992</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="O11" s="13"/>
+    </row>
+    <row r="12" spans="1:19" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="E12" s="22">
+        <v>9.7751999999999999</v>
+      </c>
+      <c r="F12" s="22">
+        <v>0.45821600000000001</v>
+      </c>
+      <c r="G12" s="22">
+        <v>0.44861400000000001</v>
+      </c>
+      <c r="I12" s="4">
+        <v>9.7911000000000001</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="O12" s="13">
+        <v>-8.1472699999999995E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="E13" s="22">
+        <v>-9.7913300000000003</v>
+      </c>
+      <c r="F13" s="22">
+        <v>-0.29977199999999998</v>
+      </c>
+      <c r="G13" s="22">
+        <v>-0.18428</v>
+      </c>
+      <c r="I13" s="4">
+        <v>9.8048699999999993</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="O13" s="13"/>
+    </row>
+    <row r="14" spans="1:19" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="I14" s="4">
+        <v>9.7941699999999994</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="O14" s="13">
+        <v>1.55627E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="I15" s="4">
+        <v>9.7825000000000006</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="O15" s="13"/>
+    </row>
+    <row r="17" spans="4:17" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="I17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="Q17" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="4:17" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="D18" s="10"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="I18" s="4">
+        <v>9.7957699999999992</v>
+      </c>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="Q18" s="13">
+        <v>-0.488037</v>
+      </c>
+    </row>
+    <row r="19" spans="4:17" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="D19" s="10"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="I19" s="4">
+        <v>9.7911000000000001</v>
+      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="Q19" s="13"/>
+    </row>
+    <row r="20" spans="4:17" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="D20" s="10"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="I20" s="4">
+        <v>9.8048699999999993</v>
+      </c>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="Q20" s="13">
+        <v>-8.1472699999999995E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="4:17" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="D21" s="10"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="I21" s="4">
+        <v>9.7941699999999994</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="Q21" s="13"/>
+    </row>
+    <row r="22" spans="4:17" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="D22" s="10"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="I22" s="4">
+        <v>9.7825000000000006</v>
+      </c>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="Q22" s="13">
+        <v>1.55627E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D23" s="10"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="Q23" s="13"/>
+    </row>
+    <row r="24" spans="4:17" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="D24" s="10"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="I24" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+    </row>
+    <row r="25" spans="4:17" ht="21.75" x14ac:dyDescent="0.25">
+      <c r="I25" s="13">
+        <v>1.0043200000000001</v>
+      </c>
+      <c r="J25" s="15">
+        <v>-2.4664700000000001E-2</v>
+      </c>
+      <c r="K25" s="15">
+        <v>-7.3756299999999997E-2</v>
+      </c>
+      <c r="Q25" s="21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="I26" s="13"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="Q26" s="13">
+        <v>-5.5873600000000002E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="I27" s="15">
+        <v>1.77276E-2</v>
+      </c>
+      <c r="J27" s="13">
+        <v>1.01322</v>
+      </c>
+      <c r="K27" s="15">
+        <v>-8.9172399999999999E-2</v>
+      </c>
+      <c r="Q27" s="13"/>
+    </row>
+    <row r="28" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="I28" s="15"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="15"/>
+      <c r="Q28" s="13">
+        <v>-0.35741000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="I29" s="15">
+        <v>7.9669599999999993E-2</v>
+      </c>
+      <c r="J29" s="15">
+        <v>8.6447399999999994E-2</v>
+      </c>
+      <c r="K29" s="13">
+        <v>0.99275000000000002</v>
+      </c>
+      <c r="Q29" s="13"/>
+    </row>
+    <row r="30" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="13"/>
+      <c r="Q30" s="13">
+        <v>0.33792899999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="Q31" s="13"/>
+    </row>
+    <row r="32" spans="4:17" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="I32" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+    </row>
+    <row r="33" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I33" s="12">
+        <v>0.22670999999999999</v>
+      </c>
+      <c r="J33" s="15">
+        <v>7.3366799999999996E-2</v>
+      </c>
+      <c r="K33" s="15">
+        <v>0.97174199999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I34" s="14"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+    </row>
+    <row r="35" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I35" s="15">
+        <v>0.60661699999999996</v>
+      </c>
+      <c r="J35" s="13">
+        <v>0.78720000000000001</v>
+      </c>
+      <c r="K35" s="16">
+        <v>-0.19672799999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I36" s="15"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="15"/>
+    </row>
+    <row r="37" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I37" s="15">
+        <v>-0.77197099999999996</v>
+      </c>
+      <c r="J37" s="15">
+        <v>0.64002899999999996</v>
+      </c>
+      <c r="K37" s="13">
+        <v>0.126337</v>
+      </c>
+    </row>
+    <row r="38" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="13"/>
+    </row>
+    <row r="39" spans="9:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+    </row>
+    <row r="40" spans="9:17" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+    </row>
+    <row r="41" spans="9:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+    </row>
+    <row r="42" spans="9:17" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
+      <c r="Q42" s="21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="9:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I43" s="18"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="18"/>
+      <c r="Q43" s="13">
+        <v>-5.5873600000000002E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="9:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="Q44" s="13"/>
+    </row>
+    <row r="45" spans="9:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="Q45" s="13">
+        <v>-0.35741000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="9:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="Q46" s="13"/>
+    </row>
+    <row r="47" spans="9:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="Q47" s="13">
+        <v>0.33792899999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="9:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="Q48" s="13"/>
+    </row>
+    <row r="49" spans="6:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="10"/>
+    </row>
+    <row r="50" spans="6:17" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="10"/>
+      <c r="Q50" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="6:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="10"/>
+      <c r="Q51" s="13">
+        <v>-0.488037</v>
+      </c>
+    </row>
+    <row r="52" spans="6:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="10"/>
+      <c r="Q52" s="13"/>
+    </row>
+    <row r="53" spans="6:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="10"/>
+      <c r="Q53" s="13">
+        <v>-8.1472699999999995E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="6:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="18"/>
+      <c r="J54" s="18"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="10"/>
+      <c r="Q54" s="13"/>
+    </row>
+    <row r="55" spans="6:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="10"/>
+      <c r="Q55" s="13">
+        <v>1.55627E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="6:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="10"/>
+      <c r="L56" s="10"/>
+      <c r="Q56" s="13"/>
+    </row>
+    <row r="57" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10"/>
+      <c r="K57" s="10"/>
+      <c r="L57" s="10"/>
+    </row>
+    <row r="58" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="10"/>
+      <c r="K58" s="10"/>
+      <c r="L58" s="10"/>
+    </row>
+    <row r="59" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="10"/>
+      <c r="K59" s="10"/>
+      <c r="L59" s="10"/>
+    </row>
+    <row r="60" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="10"/>
+      <c r="K60" s="10"/>
+      <c r="L60" s="10"/>
+    </row>
+    <row r="61" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="10"/>
+      <c r="K61" s="10"/>
+      <c r="L61" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="73">
+    <mergeCell ref="Q51:Q52"/>
+    <mergeCell ref="Q53:Q54"/>
+    <mergeCell ref="Q55:Q56"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="Q26:Q27"/>
+    <mergeCell ref="Q28:Q29"/>
+    <mergeCell ref="Q30:Q31"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="Q47:Q48"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q22:Q23"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="Q43:Q44"/>
+    <mergeCell ref="Q45:Q46"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="K37:K38"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="D1:D6"/>
     <mergeCell ref="M6:O6"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="I3:K3"/>
@@ -737,9 +1492,6 @@
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="M4:O4"/>
     <mergeCell ref="M5:O5"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="D1:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="70" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>